<commit_message>
Update 3: Fixed and Completed all functional test cases
</commit_message>
<xml_diff>
--- a/Class12/Class12Capstone/Self Learning Testcases and Results/TCSelfLearning.xlsx
+++ b/Class12/Class12Capstone/Self Learning Testcases and Results/TCSelfLearning.xlsx
@@ -16,20 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t xml:space="preserve"> Assumptions:</t>
   </si>
   <si>
-    <t>Google chrome browser is installed and opened on windows surface</t>
-  </si>
-  <si>
-    <t>The website is connected to the server with internet</t>
-  </si>
-  <si>
-    <t>User knows how to navigate the website and add new veteranian</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Test Scenario</t>
   </si>
   <si>
@@ -51,9 +42,6 @@
     <t>Pass/Fail</t>
   </si>
   <si>
-    <t>AC1TC12: Security test through SQL Injection</t>
-  </si>
-  <si>
     <t>Insert https://clinic.doveryai-no-proveryai.com/petclinic/vets in the address bar and press enter</t>
   </si>
   <si>
@@ -81,7 +69,16 @@
     <t>TO BE CONTINUE..</t>
   </si>
   <si>
-    <t>AC2: Security Testing with SQL Injection</t>
+    <t>AC2: Security testing through SQL Injection</t>
+  </si>
+  <si>
+    <t>SQL Injection tool (SQLMap) is installed</t>
+  </si>
+  <si>
+    <t>Spring Pet Clinic website is connected to the server</t>
+  </si>
+  <si>
+    <t>AC1TC12: SQL Injection on First Name input box</t>
   </si>
 </sst>
 </file>
@@ -706,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -724,7 +721,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -734,128 +731,124 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1"/>
+    <row r="11" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A6" t="s">
+      <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A7" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="2" t="s">
+    </row>
+    <row r="12" spans="1:7" ht="75.75" thickBot="1">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="75.75" thickBot="1">
-      <c r="A8" s="3" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A14" s="16"/>
+      <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11" t="s">
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A15" s="10"/>
+      <c r="B15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" ht="30.75" thickBot="1">
+      <c r="A16" s="16"/>
+      <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="23"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A17" s="12"/>
+      <c r="B17" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="4" t="s">
+      <c r="C17" s="25"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A12" s="16"/>
-      <c r="B12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="23"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>